<commit_message>
add const to sample xls
</commit_message>
<xml_diff>
--- a/src/app/sample.xlsx
+++ b/src/app/sample.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20325"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{0E935B2A-1E60-4527-BF67-7BBCF88A8619}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="bet_button_role" sheetId="1" r:id="rId1"/>
@@ -14,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="12">
   <si>
     <t>金币量下限</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -22,19 +23,6 @@
   <si>
     <t>金币量上限</t>
     <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>按钮1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>按钮2</t>
-  </si>
-  <si>
-    <t>按钮3</t>
-  </si>
-  <si>
-    <t>按钮4</t>
   </si>
   <si>
     <t>ID</t>
@@ -45,31 +33,42 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>button1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>button2</t>
-  </si>
-  <si>
-    <t>button3</t>
-  </si>
-  <si>
-    <t>button4</t>
-  </si>
-  <si>
     <t>low_gold</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>high_gold</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>预定义</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>const</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>one</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>two</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>three</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>four</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -139,7 +138,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -214,6 +213,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -249,6 +265,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -424,11 +457,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -437,9 +470,9 @@
     <col min="4" max="7" width="8.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -447,46 +480,28 @@
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="C2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A2" s="2" t="s">
+      <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" s="2"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" s="2">
         <v>0</v>
       </c>
@@ -496,20 +511,11 @@
       <c r="C4" s="1">
         <v>100000</v>
       </c>
-      <c r="D4" s="1">
-        <v>100</v>
-      </c>
-      <c r="E4" s="1">
-        <v>200</v>
-      </c>
-      <c r="F4" s="1">
-        <v>500</v>
-      </c>
-      <c r="G4" s="1">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A5" s="2">
         <v>1</v>
       </c>
@@ -519,20 +525,11 @@
       <c r="C5" s="1">
         <v>2000000</v>
       </c>
-      <c r="D5" s="1">
-        <v>100</v>
-      </c>
-      <c r="E5" s="1">
-        <v>500</v>
-      </c>
-      <c r="F5" s="1">
-        <v>1000</v>
-      </c>
-      <c r="G5" s="1">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A6" s="2">
         <v>2</v>
       </c>
@@ -542,20 +539,11 @@
       <c r="C6" s="1">
         <v>20000000</v>
       </c>
-      <c r="D6" s="1">
-        <v>100</v>
-      </c>
-      <c r="E6" s="1">
-        <v>1000</v>
-      </c>
-      <c r="F6" s="1">
-        <v>10000</v>
-      </c>
-      <c r="G6" s="1">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="D6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A7" s="2">
         <v>3</v>
       </c>
@@ -565,20 +553,11 @@
       <c r="C7" s="1">
         <v>-1</v>
       </c>
-      <c r="D7" s="1">
-        <v>100</v>
-      </c>
-      <c r="E7" s="1">
-        <v>10000</v>
-      </c>
-      <c r="F7" s="1">
-        <v>100000</v>
-      </c>
-      <c r="G7" s="1">
-        <v>200000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="D7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A8" s="2"/>
     </row>
   </sheetData>

</xml_diff>